<commit_message>
tidied up and tested ready for submission
</commit_message>
<xml_diff>
--- a/TestResultsAndGraphs.xlsx
+++ b/TestResultsAndGraphs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="21">
   <si>
     <t>ArraySize=20</t>
   </si>
@@ -55,6 +55,30 @@
   </si>
   <si>
     <t xml:space="preserve">Sending arrays </t>
+  </si>
+  <si>
+    <t>1 Thread</t>
+  </si>
+  <si>
+    <t>1Thread swaps</t>
+  </si>
+  <si>
+    <t>2Thread swaps</t>
+  </si>
+  <si>
+    <t>1 Thread - sort time</t>
+  </si>
+  <si>
+    <t>1 Thread - total time</t>
+  </si>
+  <si>
+    <t>2 Thread - sort time</t>
+  </si>
+  <si>
+    <t>2 Thread - total time</t>
+  </si>
+  <si>
+    <t>2 Threads</t>
   </si>
 </sst>
 </file>
@@ -320,11 +344,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="84919296"/>
-        <c:axId val="64628416"/>
+        <c:axId val="99945472"/>
+        <c:axId val="100936512"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="84919296"/>
+        <c:axId val="99945472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -333,7 +357,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64628416"/>
+        <c:crossAx val="100936512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -341,7 +365,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64628416"/>
+        <c:axId val="100936512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -376,7 +400,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84919296"/>
+        <c:crossAx val="99945472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -576,11 +600,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="89844224"/>
-        <c:axId val="96920128"/>
+        <c:axId val="105744384"/>
+        <c:axId val="106385920"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="89844224"/>
+        <c:axId val="105744384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -589,7 +613,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96920128"/>
+        <c:crossAx val="106385920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -597,7 +621,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96920128"/>
+        <c:axId val="106385920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -632,7 +656,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89844224"/>
+        <c:crossAx val="105744384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -832,11 +856,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="92820480"/>
-        <c:axId val="99971584"/>
+        <c:axId val="105744896"/>
+        <c:axId val="106388224"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="92820480"/>
+        <c:axId val="105744896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -845,7 +869,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99971584"/>
+        <c:crossAx val="106388224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -853,7 +877,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99971584"/>
+        <c:axId val="106388224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -888,7 +912,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92820480"/>
+        <c:crossAx val="105744896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1088,11 +1112,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="64314880"/>
-        <c:axId val="96924736"/>
+        <c:axId val="105745408"/>
+        <c:axId val="106644608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="64314880"/>
+        <c:axId val="105745408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1101,7 +1125,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96924736"/>
+        <c:crossAx val="106644608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1109,7 +1133,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96924736"/>
+        <c:axId val="106644608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1144,7 +1168,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64314880"/>
+        <c:crossAx val="105745408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1265,11 +1289,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="84918272"/>
-        <c:axId val="96923008"/>
+        <c:axId val="105745920"/>
+        <c:axId val="106646912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="84918272"/>
+        <c:axId val="105745920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1278,7 +1302,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96923008"/>
+        <c:crossAx val="106646912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1286,7 +1310,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96923008"/>
+        <c:axId val="106646912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1321,9 +1345,1543 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84918272"/>
+        <c:crossAx val="105745920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-NZ"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-NZ"/>
+              <a:t>ArraySize=30</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$136</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1 Thread - sort time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$137:$B$141</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$136</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1 Thread - total time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$137:$C$141</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$136</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2 Thread - sort time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$137:$E$141</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>96</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$136</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2 Thread - total time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$137:$F$141</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>119</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="136013312"/>
+        <c:axId val="141410880"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="136013312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="141410880"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="141410880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="136013312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-NZ"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-NZ"/>
+              <a:t>ArraySize=40</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$146</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1 Thread - sort time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$147:$B$151</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$146</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1 Thread - total time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$147:$C$151</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$146</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2 Thread - sort time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$147:$E$151</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>107</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$146</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2 Thread - total time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$147:$F$151</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>129</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="100006912"/>
+        <c:axId val="142483456"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="100006912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="142483456"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="142483456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="100006912"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-NZ"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-NZ"/>
+              <a:t>ArraySize=100</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$163</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1 Thread - sort time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$164:$B$168</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>68</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$163</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1 Thread - total time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$164:$C$168</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>71</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$163</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2 Thread - sort time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$164:$E$168</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>177</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>174</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>187</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$163</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2 Thread - total time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$164:$F$168</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>166</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>204</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>198</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>210</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="140857344"/>
+        <c:axId val="141283264"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="140857344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="141283264"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="141283264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="140857344"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-NZ"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-NZ"/>
+              <a:t>ArraySize=10</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$118</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>N</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$A$119:$A$123</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$118</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1 Thread - sort time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$119:$B$123</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$118</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1 Thread - total time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$119:$C$123</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>23</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$118</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1Thread swaps</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$119:$D$123</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$118</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2 Thread - sort time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$119:$E$123</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$118</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2 Thread - total time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$119:$F$123</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$118</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2Thread swaps</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$119:$G$123</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="142828032"/>
+        <c:axId val="140988928"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="142828032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="140988928"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="140988928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="142828032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-NZ"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-NZ"/>
+              <a:t>Time taken</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-NZ" baseline="0"/>
+              <a:t> by ArraySize averaged over N</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-NZ"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13552777777777777"/>
+          <c:y val="0"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$185</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1 Thread</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$186:$A$193</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$186:$B$193</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>18.600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>34.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>54.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>170</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$185</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2 Threads</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$186:$A$193</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$186:$C$193</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>65.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>86.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>163.19999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>217</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>344</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>689</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="74041024"/>
+        <c:axId val="74040448"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="74041024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="74040448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="74040448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="74041024"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1427,11 +2985,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="91369984"/>
-        <c:axId val="89079808"/>
+        <c:axId val="100003840"/>
+        <c:axId val="100938240"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="91369984"/>
+        <c:axId val="100003840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1440,7 +2998,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89079808"/>
+        <c:crossAx val="100938240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1448,7 +3006,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89079808"/>
+        <c:axId val="100938240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1483,7 +3041,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91369984"/>
+        <c:crossAx val="100003840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1596,11 +3154,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="85454336"/>
-        <c:axId val="89084416"/>
+        <c:axId val="100004864"/>
+        <c:axId val="100939968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="85454336"/>
+        <c:axId val="100004864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1609,7 +3167,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89084416"/>
+        <c:crossAx val="100939968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1617,7 +3175,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89084416"/>
+        <c:axId val="100939968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1652,7 +3210,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85454336"/>
+        <c:crossAx val="100004864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1768,11 +3326,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="91371520"/>
-        <c:axId val="86041728"/>
+        <c:axId val="100007424"/>
+        <c:axId val="105504768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="91371520"/>
+        <c:axId val="100007424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1781,7 +3339,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86041728"/>
+        <c:crossAx val="105504768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1789,7 +3347,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86041728"/>
+        <c:axId val="105504768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1824,7 +3382,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91371520"/>
+        <c:crossAx val="100007424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1940,11 +3498,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="89845248"/>
-        <c:axId val="86048064"/>
+        <c:axId val="105742336"/>
+        <c:axId val="105506496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="89845248"/>
+        <c:axId val="105742336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1953,7 +3511,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86048064"/>
+        <c:crossAx val="105506496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1961,7 +3519,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86048064"/>
+        <c:axId val="105506496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1996,7 +3554,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89845248"/>
+        <c:crossAx val="105742336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2124,11 +3682,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="64634176"/>
-        <c:axId val="64633600"/>
+        <c:axId val="105508224"/>
+        <c:axId val="105508800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="64634176"/>
+        <c:axId val="105508224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2162,12 +3720,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64633600"/>
+        <c:crossAx val="105508800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64633600"/>
+        <c:axId val="105508800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2202,7 +3760,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64634176"/>
+        <c:crossAx val="105508224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2409,11 +3967,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="84922880"/>
-        <c:axId val="64673984"/>
+        <c:axId val="105742848"/>
+        <c:axId val="105510528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="84922880"/>
+        <c:axId val="105742848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2422,7 +3980,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64673984"/>
+        <c:crossAx val="105510528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2430,7 +3988,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64673984"/>
+        <c:axId val="105510528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2465,7 +4023,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84922880"/>
+        <c:crossAx val="105742848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2672,11 +4230,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="84925952"/>
-        <c:axId val="74422464"/>
+        <c:axId val="105743360"/>
+        <c:axId val="106381312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="84925952"/>
+        <c:axId val="105743360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2685,7 +4243,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74422464"/>
+        <c:crossAx val="106381312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2693,7 +4251,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="74422464"/>
+        <c:axId val="106381312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2723,7 +4281,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84925952"/>
+        <c:crossAx val="105743360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2923,11 +4481,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="85881856"/>
-        <c:axId val="99969856"/>
+        <c:axId val="105743872"/>
+        <c:axId val="106383616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="85881856"/>
+        <c:axId val="105743872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2936,7 +4494,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99969856"/>
+        <c:crossAx val="106383616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2944,7 +4502,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99969856"/>
+        <c:axId val="106383616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2979,7 +4537,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85881856"/>
+        <c:crossAx val="105743872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3393,6 +4951,156 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>244928</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>29935</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>530678</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>106135</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="20" name="Chart 19"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>272142</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>138793</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>557892</xdr:colOff>
+      <xdr:row>163</xdr:row>
+      <xdr:rowOff>24493</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="21" name="Chart 20"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>299357</xdr:colOff>
+      <xdr:row>163</xdr:row>
+      <xdr:rowOff>138793</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>585107</xdr:colOff>
+      <xdr:row>178</xdr:row>
+      <xdr:rowOff>24493</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="23" name="Chart 22"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId16"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>244928</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>111579</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>530678</xdr:colOff>
+      <xdr:row>133</xdr:row>
+      <xdr:rowOff>187779</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="24" name="Chart 23"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId17"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>830034</xdr:colOff>
+      <xdr:row>180</xdr:row>
+      <xdr:rowOff>111578</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>299357</xdr:colOff>
+      <xdr:row>202</xdr:row>
+      <xdr:rowOff>108857</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="25" name="Chart 24"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId18"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3683,10 +5391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U111"/>
+  <dimension ref="A1:U193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P24" sqref="P24"/>
+    <sheetView tabSelected="1" topLeftCell="A158" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P202" sqref="P202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3697,6 +5405,7 @@
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="16.140625" customWidth="1"/>
     <col min="7" max="7" width="17.85546875" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" customWidth="1"/>
     <col min="20" max="20" width="28.7109375" customWidth="1"/>
     <col min="21" max="21" width="23.7109375" customWidth="1"/>
   </cols>
@@ -4575,7 +6284,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>7</v>
       </c>
@@ -4589,7 +6298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>1</v>
       </c>
@@ -4604,7 +6313,7 @@
         <v>5099</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>2</v>
       </c>
@@ -4619,7 +6328,7 @@
         <v>4517</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>3</v>
       </c>
@@ -4634,7 +6343,7 @@
         <v>4242</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>4</v>
       </c>
@@ -4649,7 +6358,7 @@
         <v>4550</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>5</v>
       </c>
@@ -4664,12 +6373,12 @@
         <v>4808</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>40000</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>7</v>
       </c>
@@ -4683,7 +6392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>1</v>
       </c>
@@ -4698,7 +6407,7 @@
         <v>23160</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>2</v>
       </c>
@@ -4713,7 +6422,7 @@
         <v>17427</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>3</v>
       </c>
@@ -4728,7 +6437,7 @@
         <v>14248</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>4</v>
       </c>
@@ -4743,7 +6452,7 @@
         <v>13784</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>5</v>
       </c>
@@ -4756,6 +6465,940 @@
       </c>
       <c r="D111">
         <v>13762</v>
+      </c>
+      <c r="I111">
+        <v>43</v>
+      </c>
+      <c r="J111">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I112">
+        <v>41</v>
+      </c>
+      <c r="J112">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I113">
+        <v>33</v>
+      </c>
+      <c r="J113">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>7</v>
+      </c>
+      <c r="B118" t="s">
+        <v>16</v>
+      </c>
+      <c r="C118" t="s">
+        <v>17</v>
+      </c>
+      <c r="D118" t="s">
+        <v>14</v>
+      </c>
+      <c r="E118" t="s">
+        <v>18</v>
+      </c>
+      <c r="F118" t="s">
+        <v>19</v>
+      </c>
+      <c r="G118" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>2</v>
+      </c>
+      <c r="B119">
+        <v>17</v>
+      </c>
+      <c r="C119">
+        <v>28</v>
+      </c>
+      <c r="D119">
+        <v>3</v>
+      </c>
+      <c r="E119">
+        <v>39</v>
+      </c>
+      <c r="F119">
+        <v>57</v>
+      </c>
+      <c r="G119">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>3</v>
+      </c>
+      <c r="B120">
+        <v>17</v>
+      </c>
+      <c r="C120">
+        <v>24</v>
+      </c>
+      <c r="D120">
+        <v>3</v>
+      </c>
+      <c r="E120">
+        <v>35</v>
+      </c>
+      <c r="F120">
+        <v>57</v>
+      </c>
+      <c r="G120">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>4</v>
+      </c>
+      <c r="B121">
+        <v>18</v>
+      </c>
+      <c r="C121">
+        <v>22</v>
+      </c>
+      <c r="D121">
+        <v>3</v>
+      </c>
+      <c r="E121">
+        <v>56</v>
+      </c>
+      <c r="F121">
+        <v>78</v>
+      </c>
+      <c r="G121">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>5</v>
+      </c>
+      <c r="B122">
+        <v>20</v>
+      </c>
+      <c r="C122">
+        <v>23</v>
+      </c>
+      <c r="D122">
+        <v>3</v>
+      </c>
+      <c r="E122">
+        <v>51</v>
+      </c>
+      <c r="F122">
+        <v>75</v>
+      </c>
+      <c r="G122">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>6</v>
+      </c>
+      <c r="B123">
+        <v>21</v>
+      </c>
+      <c r="C123">
+        <v>23</v>
+      </c>
+      <c r="D123">
+        <v>3</v>
+      </c>
+      <c r="E123">
+        <v>60</v>
+      </c>
+      <c r="F123">
+        <v>80</v>
+      </c>
+      <c r="G123">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>7</v>
+      </c>
+      <c r="B127" t="s">
+        <v>16</v>
+      </c>
+      <c r="C127" t="s">
+        <v>17</v>
+      </c>
+      <c r="D127" t="s">
+        <v>14</v>
+      </c>
+      <c r="E127" t="s">
+        <v>18</v>
+      </c>
+      <c r="F127" t="s">
+        <v>19</v>
+      </c>
+      <c r="G127" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>2</v>
+      </c>
+      <c r="B128">
+        <v>16</v>
+      </c>
+      <c r="C128">
+        <v>26</v>
+      </c>
+      <c r="D128">
+        <v>3</v>
+      </c>
+      <c r="E128">
+        <v>41</v>
+      </c>
+      <c r="F128">
+        <v>67</v>
+      </c>
+      <c r="G128">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>3</v>
+      </c>
+      <c r="B129">
+        <v>17</v>
+      </c>
+      <c r="C129">
+        <v>24</v>
+      </c>
+      <c r="D129">
+        <v>3</v>
+      </c>
+      <c r="E129">
+        <v>65</v>
+      </c>
+      <c r="F129">
+        <v>88</v>
+      </c>
+      <c r="G129">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>4</v>
+      </c>
+      <c r="B130">
+        <v>20</v>
+      </c>
+      <c r="C130">
+        <v>25</v>
+      </c>
+      <c r="D130">
+        <v>3</v>
+      </c>
+      <c r="E130">
+        <v>60</v>
+      </c>
+      <c r="F130">
+        <v>82</v>
+      </c>
+      <c r="G130">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>5</v>
+      </c>
+      <c r="B131">
+        <v>24</v>
+      </c>
+      <c r="C131">
+        <v>28</v>
+      </c>
+      <c r="D131">
+        <v>3</v>
+      </c>
+      <c r="E131">
+        <v>75</v>
+      </c>
+      <c r="F131">
+        <v>99</v>
+      </c>
+      <c r="G131">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>6</v>
+      </c>
+      <c r="B132">
+        <v>26</v>
+      </c>
+      <c r="C132">
+        <v>29</v>
+      </c>
+      <c r="D132">
+        <v>3</v>
+      </c>
+      <c r="E132">
+        <v>85</v>
+      </c>
+      <c r="F132">
+        <v>108</v>
+      </c>
+      <c r="G132">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>7</v>
+      </c>
+      <c r="B136" t="s">
+        <v>16</v>
+      </c>
+      <c r="C136" t="s">
+        <v>17</v>
+      </c>
+      <c r="D136" t="s">
+        <v>14</v>
+      </c>
+      <c r="E136" t="s">
+        <v>18</v>
+      </c>
+      <c r="F136" t="s">
+        <v>19</v>
+      </c>
+      <c r="G136" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>2</v>
+      </c>
+      <c r="B137">
+        <v>24</v>
+      </c>
+      <c r="C137">
+        <v>34</v>
+      </c>
+      <c r="D137">
+        <v>5</v>
+      </c>
+      <c r="E137">
+        <v>62</v>
+      </c>
+      <c r="F137">
+        <v>88</v>
+      </c>
+      <c r="G137">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>3</v>
+      </c>
+      <c r="B138">
+        <v>27</v>
+      </c>
+      <c r="C138">
+        <v>33</v>
+      </c>
+      <c r="D138">
+        <v>5</v>
+      </c>
+      <c r="E138">
+        <v>75</v>
+      </c>
+      <c r="F138">
+        <v>98</v>
+      </c>
+      <c r="G138">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>4</v>
+      </c>
+      <c r="B139">
+        <v>26</v>
+      </c>
+      <c r="C139">
+        <v>31</v>
+      </c>
+      <c r="D139">
+        <v>5</v>
+      </c>
+      <c r="E139">
+        <v>84</v>
+      </c>
+      <c r="F139">
+        <v>107</v>
+      </c>
+      <c r="G139">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>5</v>
+      </c>
+      <c r="B140">
+        <v>33</v>
+      </c>
+      <c r="C140">
+        <v>37</v>
+      </c>
+      <c r="D140">
+        <v>5</v>
+      </c>
+      <c r="E140">
+        <v>84</v>
+      </c>
+      <c r="F140">
+        <v>106</v>
+      </c>
+      <c r="G140">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>6</v>
+      </c>
+      <c r="B141">
+        <v>40</v>
+      </c>
+      <c r="C141">
+        <v>44</v>
+      </c>
+      <c r="D141">
+        <v>5</v>
+      </c>
+      <c r="E141">
+        <v>96</v>
+      </c>
+      <c r="F141">
+        <v>119</v>
+      </c>
+      <c r="G141">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>7</v>
+      </c>
+      <c r="B146" t="s">
+        <v>16</v>
+      </c>
+      <c r="C146" t="s">
+        <v>17</v>
+      </c>
+      <c r="D146" t="s">
+        <v>14</v>
+      </c>
+      <c r="E146" t="s">
+        <v>18</v>
+      </c>
+      <c r="F146" t="s">
+        <v>19</v>
+      </c>
+      <c r="G146" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>2</v>
+      </c>
+      <c r="B147">
+        <v>31</v>
+      </c>
+      <c r="C147">
+        <v>42</v>
+      </c>
+      <c r="D147">
+        <v>7</v>
+      </c>
+      <c r="E147">
+        <v>71</v>
+      </c>
+      <c r="F147">
+        <v>97</v>
+      </c>
+      <c r="G147">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>3</v>
+      </c>
+      <c r="B148">
+        <v>30</v>
+      </c>
+      <c r="C148">
+        <v>36</v>
+      </c>
+      <c r="D148">
+        <v>6</v>
+      </c>
+      <c r="E148">
+        <v>68</v>
+      </c>
+      <c r="F148">
+        <v>88</v>
+      </c>
+      <c r="G148">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>4</v>
+      </c>
+      <c r="B149">
+        <v>33</v>
+      </c>
+      <c r="C149">
+        <v>38</v>
+      </c>
+      <c r="D149">
+        <v>7</v>
+      </c>
+      <c r="E149">
+        <v>90</v>
+      </c>
+      <c r="F149">
+        <v>114</v>
+      </c>
+      <c r="G149">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>5</v>
+      </c>
+      <c r="B150">
+        <v>39</v>
+      </c>
+      <c r="C150">
+        <v>42</v>
+      </c>
+      <c r="D150">
+        <v>6</v>
+      </c>
+      <c r="E150">
+        <v>97</v>
+      </c>
+      <c r="F150">
+        <v>119</v>
+      </c>
+      <c r="G150">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>6</v>
+      </c>
+      <c r="B151">
+        <v>40</v>
+      </c>
+      <c r="C151">
+        <v>42</v>
+      </c>
+      <c r="D151">
+        <v>6</v>
+      </c>
+      <c r="E151">
+        <v>107</v>
+      </c>
+      <c r="F151">
+        <v>129</v>
+      </c>
+      <c r="G151">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>7</v>
+      </c>
+      <c r="B155" t="s">
+        <v>16</v>
+      </c>
+      <c r="C155" t="s">
+        <v>17</v>
+      </c>
+      <c r="D155" t="s">
+        <v>14</v>
+      </c>
+      <c r="E155" t="s">
+        <v>18</v>
+      </c>
+      <c r="F155" t="s">
+        <v>19</v>
+      </c>
+      <c r="G155" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>2</v>
+      </c>
+      <c r="B156">
+        <v>33</v>
+      </c>
+      <c r="C156">
+        <v>46</v>
+      </c>
+      <c r="D156">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>3</v>
+      </c>
+      <c r="B157">
+        <v>34</v>
+      </c>
+      <c r="C157">
+        <v>42</v>
+      </c>
+      <c r="D157">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>4</v>
+      </c>
+      <c r="B158">
+        <v>37</v>
+      </c>
+      <c r="C158">
+        <v>42</v>
+      </c>
+      <c r="D158">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>5</v>
+      </c>
+      <c r="B159">
+        <v>45</v>
+      </c>
+      <c r="C159">
+        <v>48</v>
+      </c>
+      <c r="D159">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>6</v>
+      </c>
+      <c r="B160">
+        <v>69</v>
+      </c>
+      <c r="C160">
+        <v>73</v>
+      </c>
+      <c r="D160">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>7</v>
+      </c>
+      <c r="B163" t="s">
+        <v>16</v>
+      </c>
+      <c r="C163" t="s">
+        <v>17</v>
+      </c>
+      <c r="D163" t="s">
+        <v>14</v>
+      </c>
+      <c r="E163" t="s">
+        <v>18</v>
+      </c>
+      <c r="F163" t="s">
+        <v>19</v>
+      </c>
+      <c r="G163" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>2</v>
+      </c>
+      <c r="B164">
+        <v>42</v>
+      </c>
+      <c r="C164">
+        <v>55</v>
+      </c>
+      <c r="D164">
+        <v>14</v>
+      </c>
+      <c r="E164">
+        <v>140</v>
+      </c>
+      <c r="F164">
+        <v>165</v>
+      </c>
+      <c r="G164">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>3</v>
+      </c>
+      <c r="B165">
+        <v>48</v>
+      </c>
+      <c r="C165">
+        <v>55</v>
+      </c>
+      <c r="D165">
+        <v>13</v>
+      </c>
+      <c r="E165">
+        <v>138</v>
+      </c>
+      <c r="F165">
+        <v>166</v>
+      </c>
+      <c r="G165">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>4</v>
+      </c>
+      <c r="B166">
+        <v>56</v>
+      </c>
+      <c r="C166">
+        <v>60</v>
+      </c>
+      <c r="D166">
+        <v>14</v>
+      </c>
+      <c r="E166">
+        <v>177</v>
+      </c>
+      <c r="F166">
+        <v>204</v>
+      </c>
+      <c r="G166">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>5</v>
+      </c>
+      <c r="B167">
+        <v>59</v>
+      </c>
+      <c r="C167">
+        <v>62</v>
+      </c>
+      <c r="D167">
+        <v>14</v>
+      </c>
+      <c r="E167">
+        <v>174</v>
+      </c>
+      <c r="F167">
+        <v>198</v>
+      </c>
+      <c r="G167">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>6</v>
+      </c>
+      <c r="B168">
+        <v>68</v>
+      </c>
+      <c r="C168">
+        <v>71</v>
+      </c>
+      <c r="D168">
+        <v>14</v>
+      </c>
+      <c r="E168">
+        <v>187</v>
+      </c>
+      <c r="F168">
+        <v>210</v>
+      </c>
+      <c r="G168">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>8</v>
+      </c>
+      <c r="B185" t="s">
+        <v>13</v>
+      </c>
+      <c r="C185" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>10</v>
+      </c>
+      <c r="B186">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="C186">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>20</v>
+      </c>
+      <c r="B187">
+        <v>20.6</v>
+      </c>
+      <c r="C187">
+        <v>65.2</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>30</v>
+      </c>
+      <c r="B188">
+        <v>30</v>
+      </c>
+      <c r="C188">
+        <v>80.2</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>40</v>
+      </c>
+      <c r="B189">
+        <v>34.6</v>
+      </c>
+      <c r="C189">
+        <v>86.6</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>100</v>
+      </c>
+      <c r="B190">
+        <v>54.6</v>
+      </c>
+      <c r="C190">
+        <v>163.19999999999999</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>200</v>
+      </c>
+      <c r="B191">
+        <v>73</v>
+      </c>
+      <c r="C191">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>400</v>
+      </c>
+      <c r="B192">
+        <v>106</v>
+      </c>
+      <c r="C192">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>800</v>
+      </c>
+      <c r="B193">
+        <v>170</v>
+      </c>
+      <c r="C193">
+        <v>689</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final touch ups to Main.java for submission
</commit_message>
<xml_diff>
--- a/TestResultsAndGraphs.xlsx
+++ b/TestResultsAndGraphs.xlsx
@@ -85,7 +85,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,8 +119,16 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -137,8 +145,25 @@
         <fgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -213,13 +238,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
@@ -244,8 +287,14 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="3"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="6">
+    <cellStyle name="40% - Accent1" xfId="4" builtinId="31"/>
+    <cellStyle name="40% - Accent2" xfId="5" builtinId="35"/>
+    <cellStyle name="Check Cell" xfId="3" builtinId="23"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="2" builtinId="10"/>
@@ -275,7 +324,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -344,11 +392,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="99945472"/>
-        <c:axId val="100936512"/>
+        <c:axId val="136315392"/>
+        <c:axId val="123632384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="99945472"/>
+        <c:axId val="136315392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -357,7 +405,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100936512"/>
+        <c:crossAx val="123632384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -365,7 +413,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100936512"/>
+        <c:axId val="123632384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -393,21 +441,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99945472"/>
+        <c:crossAx val="136315392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -600,11 +646,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="105744384"/>
-        <c:axId val="106385920"/>
+        <c:axId val="46259200"/>
+        <c:axId val="46719552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="105744384"/>
+        <c:axId val="46259200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -613,7 +659,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106385920"/>
+        <c:crossAx val="46719552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -621,7 +667,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106385920"/>
+        <c:axId val="46719552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -656,7 +702,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105744384"/>
+        <c:crossAx val="46259200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -856,11 +902,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="105744896"/>
-        <c:axId val="106388224"/>
+        <c:axId val="46259712"/>
+        <c:axId val="46721856"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="105744896"/>
+        <c:axId val="46259712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -869,7 +915,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106388224"/>
+        <c:crossAx val="46721856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -877,7 +923,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106388224"/>
+        <c:axId val="46721856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -912,7 +958,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105744896"/>
+        <c:crossAx val="46259712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1112,11 +1158,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="105745408"/>
-        <c:axId val="106644608"/>
+        <c:axId val="46878720"/>
+        <c:axId val="46724160"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="105745408"/>
+        <c:axId val="46878720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1125,7 +1171,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106644608"/>
+        <c:crossAx val="46724160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1133,7 +1179,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106644608"/>
+        <c:axId val="46724160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1168,7 +1214,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105745408"/>
+        <c:crossAx val="46878720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1220,7 +1266,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1289,11 +1334,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="105745920"/>
-        <c:axId val="106646912"/>
+        <c:axId val="46879232"/>
+        <c:axId val="46726464"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="105745920"/>
+        <c:axId val="46879232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1302,7 +1347,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106646912"/>
+        <c:crossAx val="46726464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1310,7 +1355,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106646912"/>
+        <c:axId val="46726464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1338,21 +1383,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105745920"/>
+        <c:crossAx val="46879232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1392,7 +1435,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-NZ"/>
-              <a:t>ArraySize=30</a:t>
+              <a:t>ArraySize=30 vs. N=2..6</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1450,51 +1493,8 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="4"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$C$136</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>1 Thread - total time</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$137:$C$141</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>37</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>44</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$E$136</c:f>
@@ -1529,49 +1529,6 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>96</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$F$136</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>2 Thread - total time</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$F$137:$F$141</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>88</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>98</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>107</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>106</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>119</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1588,11 +1545,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="136013312"/>
-        <c:axId val="141410880"/>
+        <c:axId val="46879744"/>
+        <c:axId val="47129728"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="136013312"/>
+        <c:axId val="46879744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1601,7 +1558,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141410880"/>
+        <c:crossAx val="47129728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1609,7 +1566,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="141410880"/>
+        <c:axId val="47129728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1617,6 +1574,26 @@
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NZ"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-NZ" baseline="0"/>
+                  <a:t> (ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-NZ"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
@@ -1624,7 +1601,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136013312"/>
+        <c:crossAx val="46879744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1671,7 +1648,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-NZ"/>
-              <a:t>ArraySize=40</a:t>
+              <a:t>ArraySize=40 vs. N=2..6</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1729,51 +1706,8 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="4"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$C$146</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>1 Thread - total time</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$147:$C$151</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>42</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$E$146</c:f>
@@ -1808,49 +1742,6 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>107</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$F$146</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>2 Thread - total time</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$F$147:$F$151</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>97</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>88</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>114</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>119</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>129</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1867,11 +1758,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="100006912"/>
-        <c:axId val="142483456"/>
+        <c:axId val="46880768"/>
+        <c:axId val="47132032"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="100006912"/>
+        <c:axId val="46880768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1880,7 +1771,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142483456"/>
+        <c:crossAx val="47132032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1888,7 +1779,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142483456"/>
+        <c:axId val="47132032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1896,6 +1787,26 @@
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NZ"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-NZ" baseline="0"/>
+                  <a:t> (ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-NZ"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
@@ -1903,7 +1814,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100006912"/>
+        <c:crossAx val="46880768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1956,7 +1867,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-NZ"/>
-              <a:t>ArraySize=100</a:t>
+              <a:t>ArraySize=100 vs. N=2..6</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2014,51 +1925,8 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="4"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$C$163</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>1 Thread - total time</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$164:$C$168</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>62</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>71</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$E$163</c:f>
@@ -2093,49 +1961,6 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>187</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$F$163</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>2 Thread - total time</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$F$164:$F$168</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>165</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>166</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>204</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>198</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>210</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2152,11 +1977,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="140857344"/>
-        <c:axId val="141283264"/>
+        <c:axId val="46880256"/>
+        <c:axId val="47135488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="140857344"/>
+        <c:axId val="46880256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2165,7 +1990,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141283264"/>
+        <c:crossAx val="47135488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2173,7 +1998,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="141283264"/>
+        <c:axId val="47135488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2181,6 +2006,26 @@
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NZ"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-NZ" baseline="0"/>
+                  <a:t> (ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-NZ"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
@@ -2188,7 +2033,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140857344"/>
+        <c:crossAx val="46880256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2235,7 +2080,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-NZ"/>
-              <a:t>ArraySize=10</a:t>
+              <a:t>ArraySize=10 vs. N=2..6</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2250,51 +2095,8 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$118</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>N</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$A$119:$A$123</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$B$118</c:f>
@@ -2336,94 +2138,8 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$C$118</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>1 Thread - total time</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$119:$C$123</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>23</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$D$118</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>1Thread swaps</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$119:$D$123</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
           <c:idx val="4"/>
-          <c:order val="4"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$E$118</c:f>
@@ -2458,92 +2174,6 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>60</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$F$118</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>2 Thread - total time</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$F$119:$F$123</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>57</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>57</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>78</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>80</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$G$118</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>2Thread swaps</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$G$119:$G$123</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2560,11 +2190,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="142828032"/>
-        <c:axId val="140988928"/>
+        <c:axId val="47419392"/>
+        <c:axId val="47679168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="142828032"/>
+        <c:axId val="47419392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2573,7 +2203,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140988928"/>
+        <c:crossAx val="47679168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2581,7 +2211,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="140988928"/>
+        <c:axId val="47679168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2589,6 +2219,21 @@
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NZ"/>
+                  <a:t>Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
@@ -2596,7 +2241,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142828032"/>
+        <c:crossAx val="47419392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2647,7 +2292,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-NZ" baseline="0"/>
-              <a:t> by ArraySize averaged over N</a:t>
+              <a:t> by ArraySize for N=3</a:t>
             </a:r>
             <a:endParaRPr lang="en-NZ"/>
           </a:p>
@@ -2685,32 +2330,26 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$186:$A$193</c:f>
+              <c:f>Sheet1!$A$186:$A$191</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="7">
                   <c:v>800</c:v>
                 </c:pt>
               </c:numCache>
@@ -2718,32 +2357,26 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$186:$B$193</c:f>
+              <c:f>Sheet1!$B$186:$B$191</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>18.600000000000001</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.6</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>34.6</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>54.6</c:v>
+                  <c:v>106</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>73</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>106</c:v>
-                </c:pt>
-                <c:pt idx="7">
                   <c:v>170</c:v>
                 </c:pt>
               </c:numCache>
@@ -2767,32 +2400,26 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$186:$A$193</c:f>
+              <c:f>Sheet1!$A$186:$A$191</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="7">
                   <c:v>800</c:v>
                 </c:pt>
               </c:numCache>
@@ -2800,32 +2427,26 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$186:$C$193</c:f>
+              <c:f>Sheet1!$C$186:$C$191</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>48</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>65.2</c:v>
+                  <c:v>103</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>80.2</c:v>
+                  <c:v>153</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>86.6</c:v>
+                  <c:v>217</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>163.19999999999999</c:v>
+                  <c:v>344</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>217</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>344</c:v>
-                </c:pt>
-                <c:pt idx="7">
                   <c:v>689</c:v>
                 </c:pt>
               </c:numCache>
@@ -2841,17 +2462,32 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="74041024"/>
-        <c:axId val="74040448"/>
+        <c:axId val="47681472"/>
+        <c:axId val="47682048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="74041024"/>
+        <c:axId val="47681472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NZ"/>
+                  <a:t>ArraySize</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
@@ -2859,12 +2495,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74040448"/>
+        <c:crossAx val="47682048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="74040448"/>
+        <c:axId val="47682048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2872,6 +2508,26 @@
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NZ"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-NZ" baseline="0"/>
+                  <a:t> (ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-NZ"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
@@ -2879,9 +2535,222 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74041024"/>
+        <c:crossAx val="47681472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-NZ"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-NZ"/>
+              <a:t>ArraySize=20 vs. N=2..6</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$127</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1 Thread - sort time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$128:$B$132</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$127</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2 Thread - sort time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$128:$E$132</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>85</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="68146688"/>
+        <c:axId val="151988480"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="68146688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="151988480"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="151988480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NZ"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-NZ" baseline="0"/>
+                  <a:t> (ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-NZ"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="68146688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2916,7 +2785,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2985,11 +2853,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="100003840"/>
-        <c:axId val="100938240"/>
+        <c:axId val="46256128"/>
+        <c:axId val="46547520"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="100003840"/>
+        <c:axId val="46256128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2998,7 +2866,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100938240"/>
+        <c:crossAx val="46547520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3006,7 +2874,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100938240"/>
+        <c:axId val="46547520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3034,21 +2902,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100003840"/>
+        <c:crossAx val="46256128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:ln>
@@ -3085,7 +2951,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3154,11 +3019,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="100004864"/>
-        <c:axId val="100939968"/>
+        <c:axId val="46256640"/>
+        <c:axId val="46549248"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="100004864"/>
+        <c:axId val="46256640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3167,7 +3032,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100939968"/>
+        <c:crossAx val="46549248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3175,7 +3040,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100939968"/>
+        <c:axId val="46549248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3203,21 +3068,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100004864"/>
+        <c:crossAx val="46256640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3247,7 +3110,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3326,11 +3188,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="100007424"/>
-        <c:axId val="105504768"/>
+        <c:axId val="46257152"/>
+        <c:axId val="46550976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="100007424"/>
+        <c:axId val="46257152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3339,7 +3201,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105504768"/>
+        <c:crossAx val="46550976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3347,7 +3209,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105504768"/>
+        <c:axId val="46550976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3375,21 +3237,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100007424"/>
+        <c:crossAx val="46257152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3419,7 +3279,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3498,11 +3357,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="105742336"/>
-        <c:axId val="105506496"/>
+        <c:axId val="136315904"/>
+        <c:axId val="46552704"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="105742336"/>
+        <c:axId val="136315904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3511,7 +3370,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105506496"/>
+        <c:crossAx val="46552704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3519,7 +3378,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105506496"/>
+        <c:axId val="46552704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3547,21 +3406,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105742336"/>
+        <c:crossAx val="136315904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3606,7 +3463,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3682,11 +3538,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="105508224"/>
-        <c:axId val="105508800"/>
+        <c:axId val="46554432"/>
+        <c:axId val="46497792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="105508224"/>
+        <c:axId val="46554432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3713,19 +3569,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105508800"/>
+        <c:crossAx val="46497792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="105508800"/>
+        <c:axId val="46497792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3753,21 +3608,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105508224"/>
+        <c:crossAx val="46554432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3812,7 +3665,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3967,11 +3819,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="105742848"/>
-        <c:axId val="105510528"/>
+        <c:axId val="46257664"/>
+        <c:axId val="46499520"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="105742848"/>
+        <c:axId val="46257664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3980,7 +3832,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105510528"/>
+        <c:crossAx val="46499520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3988,7 +3840,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105510528"/>
+        <c:axId val="46499520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4016,21 +3868,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105742848"/>
+        <c:crossAx val="46257664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4075,7 +3925,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4230,11 +4079,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="105743360"/>
-        <c:axId val="106381312"/>
+        <c:axId val="46258176"/>
+        <c:axId val="46501824"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="105743360"/>
+        <c:axId val="46258176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4243,7 +4092,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106381312"/>
+        <c:crossAx val="46501824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4251,7 +4100,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106381312"/>
+        <c:axId val="46501824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4274,21 +4123,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105743360"/>
+        <c:crossAx val="46258176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4481,11 +4328,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="105743872"/>
-        <c:axId val="106383616"/>
+        <c:axId val="46258688"/>
+        <c:axId val="46504128"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="105743872"/>
+        <c:axId val="46258688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4494,7 +4341,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106383616"/>
+        <c:crossAx val="46504128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4502,7 +4349,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106383616"/>
+        <c:axId val="46504128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4537,7 +4384,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105743872"/>
+        <c:crossAx val="46258688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4954,15 +4801,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>244928</xdr:colOff>
-      <xdr:row>134</xdr:row>
-      <xdr:rowOff>29935</xdr:rowOff>
+      <xdr:colOff>285749</xdr:colOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>166007</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>530678</xdr:colOff>
-      <xdr:row>148</xdr:row>
-      <xdr:rowOff>106135</xdr:rowOff>
+      <xdr:colOff>571499</xdr:colOff>
+      <xdr:row>135</xdr:row>
+      <xdr:rowOff>51707</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4983,15 +4830,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>272142</xdr:colOff>
-      <xdr:row>148</xdr:row>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>598714</xdr:colOff>
+      <xdr:row>120</xdr:row>
       <xdr:rowOff>138793</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>557892</xdr:colOff>
-      <xdr:row>163</xdr:row>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>802821</xdr:colOff>
+      <xdr:row>135</xdr:row>
       <xdr:rowOff>24493</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5014,15 +4861,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>299357</xdr:colOff>
-      <xdr:row>163</xdr:row>
-      <xdr:rowOff>138793</xdr:rowOff>
+      <xdr:colOff>312964</xdr:colOff>
+      <xdr:row>137</xdr:row>
+      <xdr:rowOff>97972</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>585107</xdr:colOff>
-      <xdr:row>178</xdr:row>
-      <xdr:rowOff>24493</xdr:rowOff>
+      <xdr:colOff>598714</xdr:colOff>
+      <xdr:row>151</xdr:row>
+      <xdr:rowOff>174172</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5045,14 +4892,14 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>244928</xdr:colOff>
-      <xdr:row>119</xdr:row>
-      <xdr:rowOff>111579</xdr:rowOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>125187</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>530678</xdr:colOff>
-      <xdr:row>133</xdr:row>
-      <xdr:rowOff>187779</xdr:rowOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>10887</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5096,6 +4943,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId18"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>585106</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>789213</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId19"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5391,14 +5268,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U193"/>
+  <dimension ref="A1:U191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A158" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P202" sqref="P202"/>
+    <sheetView tabSelected="1" topLeftCell="G101" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B198" sqref="B198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="17.5703125" customWidth="1"/>
@@ -7302,102 +7180,81 @@
         <v>8</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
+    <row r="184" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="185" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A185" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B185" t="s">
+      <c r="B185" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C185" t="s">
+      <c r="C185" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A186">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B186">
-        <v>18.600000000000001</v>
+        <v>59</v>
       </c>
       <c r="C186">
-        <v>48</v>
+        <v>72</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="B187">
-        <v>20.6</v>
+        <v>61</v>
       </c>
       <c r="C187">
-        <v>65.2</v>
+        <v>103</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="B188">
-        <v>30</v>
+        <v>73</v>
       </c>
       <c r="C188">
-        <v>80.2</v>
+        <v>153</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189">
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="B189">
-        <v>34.6</v>
+        <v>73</v>
       </c>
       <c r="C189">
-        <v>86.6</v>
+        <v>217</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="B190">
-        <v>54.6</v>
+        <v>106</v>
       </c>
       <c r="C190">
-        <v>163.19999999999999</v>
+        <v>344</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191">
-        <v>200</v>
+        <v>800</v>
       </c>
       <c r="B191">
-        <v>73</v>
+        <v>170</v>
       </c>
       <c r="C191">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A192">
-        <v>400</v>
-      </c>
-      <c r="B192">
-        <v>106</v>
-      </c>
-      <c r="C192">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A193">
-        <v>800</v>
-      </c>
-      <c r="B193">
-        <v>170</v>
-      </c>
-      <c r="C193">
         <v>689</v>
       </c>
     </row>

</xml_diff>